<commit_message>
Dev: Move file resource
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BARA\Documents\UiPath\SignedInvoiceStoring\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192550B3-9E67-42A0-8979-6DD0FA3EB4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85656C19-0AB1-4AE5-B4BB-C807F19B8EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>STR_FOLDER_PATH</t>
-  </si>
-  <si>
     <t>use in Main-&gt; Initialization</t>
   </si>
   <si>
@@ -226,6 +223,88 @@
   </si>
   <si>
     <t>For Get the secret of the connection string.</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>strINVOICE_LM_STATUS_Column</t>
+  </si>
+  <si>
+    <t>strInvoiceValidStatus</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>log_validInvoiceProcessing</t>
+  </si>
+  <si>
+    <t>Processing Valid-Invoice ID:</t>
+  </si>
+  <si>
+    <t>Bookmark: Log Message log_validInvoiceProcessing</t>
+  </si>
+  <si>
+    <t>logE_UnexpectedDiverseKey</t>
+  </si>
+  <si>
+    <t>Unexpected dictInvoiceFileSetForInsert/currentKeyValuePairOfTextAndDataRow diverse key.</t>
+  </si>
+  <si>
+    <t>Bookmark: Throw logE_UnexpectedDiverseKey</t>
+  </si>
+  <si>
+    <t>declare @ResultCode nvarchar(10)
+	,@ResultMessages NVARCHAR(MAX)
+EXECUTE [dbo].[UPLOAD_AND_UPDATE_APPROVED_INVOICE] 
+   @INVOICE_ID = @IN_INVOICE_ID
+  ,@BASE64 = @IN_BASE64
+  ,@ResultCode OUTPUT
+  ,@ResultMessages OUTPUT
+SELECT @ResultCode AS RESULT_CODE , @ResultMessages as RESULT_MESSAGES</t>
+  </si>
+  <si>
+    <t>strQueryUploadInvoice</t>
+  </si>
+  <si>
+    <t>Bookmark: Run Query Upload Invoice
+Query Parameters:
+IN_INVOICE_ID = INVOICE_ID of the invoice.
+IN_BASE64 = converted base64 of the invoice file.
+Required output:
+RESULT_CODE
+RESULT_MESSAGES</t>
+  </si>
+  <si>
+    <t>logE_UnexpectedQueryResult</t>
+  </si>
+  <si>
+    <t>The updated file to SQL Server was not affected, Invoice No. @INVOICE_NO, Invoice ID @INVOICE_ID</t>
+  </si>
+  <si>
+    <t>Bookmark: Throw logE_UnexpectedQueryResult
+Parameter:
+@INVOICE_ID
+@INVOICE_NO</t>
+  </si>
+  <si>
+    <t>Update Successfully</t>
+  </si>
+  <si>
+    <t>log_successfullyUpdatedToSQL</t>
+  </si>
+  <si>
+    <t>Bookmark: Log Message log_successfullyUpdatedToSQL</t>
+  </si>
+  <si>
+    <t>strRawFilesFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\BARA\Documents\UCL_F</t>
+  </si>
+  <si>
+    <t>strFinishProcessedFilesFolderPath</t>
   </si>
 </sst>
 </file>
@@ -283,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -305,6 +384,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -675,7 +757,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -686,7 +768,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>32</v>
@@ -697,10 +779,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="30">
@@ -716,89 +798,160 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="8" spans="1:26" ht="45">
-      <c r="A8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="45">
       <c r="A9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>63</v>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60">
+      <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="165">
+      <c r="A21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1765,6 +1918,9 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1903,10 +2059,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1956,7 +2112,7 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17">
         <v>2</v>

</xml_diff>